<commit_message>
momdificacion de casos de uso
</commit_message>
<xml_diff>
--- a/trunk/docs/Entregables/Casos%20de%20uso%20de%20negocio/Casos de Test Backend - V1.xlsx
+++ b/trunk/docs/Entregables/Casos%20de%20uso%20de%20negocio/Casos de Test Backend - V1.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jcaro\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmont3\Downloads\UTN\Proyecto\SAFE\trunk\docs\Entregables\Casos%20de%20uso%20de%20negocio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7830" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15330" windowHeight="7830"/>
   </bookViews>
   <sheets>
     <sheet name="Alumno" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>FiltrosAlumno</t>
   </si>
   <si>
-    <t>Ingresar datos en los filtros de búsqueda para encontrar los Alumnoes que cumplan con las condiciones ingresadas</t>
-  </si>
-  <si>
     <t>Que se visualicen los Alumnoes que coincidan los datos con los ingresados</t>
   </si>
   <si>
@@ -261,12 +258,15 @@
   </si>
   <si>
     <t>Que permita ingresar únicamente 10 digitos en el campo de Documento</t>
+  </si>
+  <si>
+    <t>Ingresar datos en los filtros de búsqueda para encontrar los Alumnos que cumplan con las condiciones ingresadas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -399,7 +399,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -474,6 +474,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -509,6 +526,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -663,11 +697,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.5703125" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
@@ -714,10 +748,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
@@ -740,16 +774,16 @@
     </row>
     <row r="5" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C5" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>21</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>22</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
@@ -761,40 +795,40 @@
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>15</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>18</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>9</v>
@@ -804,48 +838,48 @@
     </row>
     <row r="9" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>26</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>27</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>29</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>30</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:6" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -924,11 +958,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="36" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:27" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -983,29 +1017,29 @@
     </row>
     <row r="3" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>36</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
@@ -1015,112 +1049,112 @@
     </row>
     <row r="5" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>40</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>41</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:27" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>48</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:27" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
     </row>
     <row r="11" spans="1:27" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>53</v>
       </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -1138,7 +1172,7 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
     <col min="3" max="3" width="40.5703125" customWidth="1"/>
@@ -1199,29 +1233,29 @@
     </row>
     <row r="3" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>58</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
@@ -1231,96 +1265,96 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>64</v>
       </c>
       <c r="E5" s="10"/>
       <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:26" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>66</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>67</v>
       </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>69</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>70</v>
       </c>
       <c r="E7" s="10"/>
       <c r="F7" s="6"/>
     </row>
     <row r="8" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>77</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>78</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:26" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="10" t="s">
-        <v>72</v>
-      </c>
       <c r="D9" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>74</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>75</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>

</xml_diff>